<commit_message>
update reverse search func
</commit_message>
<xml_diff>
--- a/memes_top5.xlsx
+++ b/memes_top5.xlsx
@@ -517,33 +517,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/memes/comments/1pdjswx/protect_him_at_all_costs/</t>
+          <t>https://www.reddit.com/r/memes/comments/1peh1jx/its_good_i_guess/</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://i.redd.it/v29qg0yrn25g1.jpeg</t>
+          <t>https://i.redd.it/7m9gztd38a5g1.jpeg</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>32379</v>
+        <v>40172</v>
       </c>
       <c r="D2" t="n">
-        <v>616</v>
+        <v>272</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>music and celebrity culture,fandom in-joke,gender stereotypes,culture war discourse,job or class stereotypes,anti-societal</t>
+          <t>social awkwardness,tv and movie reference,chaotic low-effort meme,referential meme,cross-cultural misunderstanding,work or school niche meme</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>music and celebrity culture:41.84%,fandom in-joke:40.99%,gender stereotypes:39.39%,culture war discourse:38.30%,job or class stereotypes:37.48%,anti-societal:36.88%</t>
+          <t>social awkwardness:45.49%,tv and movie reference:38.29%,chaotic low-effort meme:38.16%,referential meme:35.83%,cross-cultural misunderstanding:35.71%,work or school niche meme:35.04%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -555,57 +555,57 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/memes/comments/1pdw0ag/double_standards/</t>
+          <t>https://www.reddit.com/r/memes/comments/1peha3a/havent_used_mine_in_18_months/</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://i.redd.it/a99yc8ehs55g1.jpeg</t>
+          <t>https://i.redd.it/cpomq8u1aa5g1.jpeg</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>31419</v>
+        <v>27617</v>
       </c>
       <c r="D3" t="n">
-        <v>509</v>
+        <v>2153</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>genre-reactionary,animal reaction meme,referential meme,abstract or bizarre humour,animals acting like humans,funny pet behaviour</t>
+          <t>personal stories and situations,everyday inconveniences,work or school niche meme,music and celebrity culture,referential meme,internet niche meme</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>genre-reactionary:45.13%,animal reaction meme:44.58%,referential meme:43.50%,abstract or bizarre humour:43.38%,animals acting like humans:42.45%,funny pet behaviour:42.33%</t>
+          <t>personal stories and situations:40.29%,everyday inconveniences:39.49%,work or school niche meme:34.64%,music and celebrity culture:33.37%,referential meme:32.74%,internet niche meme:32.68%</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>mostly larger</t>
+          <t>mostly smaller</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/memes/comments/1pdb1s1/they_keep_folding_it_further_man/</t>
+          <t>https://www.reddit.com/r/memes/comments/1peg5a7/just_a_quick_trip/</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://i.redd.it/wdlamvzy015g1.png</t>
+          <t>https://i.redd.it/536z12131a5g1.jpeg</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>26379</v>
+        <v>15364</v>
       </c>
       <c r="D4" t="n">
-        <v>409</v>
+        <v>128</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -614,12 +614,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>everyday inconveniences,genre-reactionary,music and celebrity culture,abstract or bizarre humour,global north vs global south,chaotic low-effort meme</t>
+          <t>chaotic low-effort meme,referential meme,internet niche meme,historical figure in modern setting,tv and movie reference,abstract or bizarre humour</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>everyday inconveniences:22.59%,genre-reactionary:19.48%,music and celebrity culture:19.03%,abstract or bizarre humour:18.74%,global north vs global south:17.44%,chaotic low-effort meme:17.01%</t>
+          <t>chaotic low-effort meme:49.19%,referential meme:47.97%,internet niche meme:46.31%,historical figure in modern setting:45.93%,tv and movie reference:45.43%,abstract or bizarre humour:44.74%</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -631,19 +631,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/memes/comments/1pdy2c5/way_down_we_go/</t>
+          <t>https://www.reddit.com/r/memes/comments/1pepp0n/what_its_like_to_solve_trigonometry_problems/</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/tufn98a4hc5g1.png</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>11001</v>
+        <v>9395</v>
       </c>
       <c r="D5" t="n">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -652,36 +652,36 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>historical figure in modern setting,abstract or bizarre humour,chaotic low-effort meme,anime and fandom reference,referential meme,internet niche meme</t>
+          <t>chaotic low-effort meme,internet niche meme,abstract or bizarre humour,tv and movie reference,historical figure in modern setting,referential meme</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>historical figure in modern setting:43.10%,abstract or bizarre humour:42.92%,chaotic low-effort meme:40.98%,anime and fandom reference:40.84%,referential meme:38.46%,internet niche meme:36.92%</t>
+          <t>chaotic low-effort meme:40.98%,internet niche meme:40.28%,abstract or bizarre humour:39.41%,tv and movie reference:36.71%,historical figure in modern setting:36.32%,referential meme:35.96%</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>mixed</t>
+          <t>mostly larger</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/memes/comments/1pdcsfu/dinner_is_cooked_lets_eat/</t>
+          <t>https://www.reddit.com/r/memes/comments/1pen392/why_ram_prices_shooting_up_lately/</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://i.redd.it/eqlv3h9rb15g1.png</t>
+          <t>https://i.redd.it/n77t88wpob5g1.jpeg</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5965</v>
+        <v>6080</v>
       </c>
       <c r="D6" t="n">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -690,17 +690,17 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>relationships and social life relatability,personal stories and situations,fandom in-joke,tv and movie reference,animals acting like humans,abstract or bizarre humour</t>
+          <t>funny pet behaviour,personal stories and situations,genre-reactionary,animals acting like humans,chaotic low-effort meme,referential meme</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>relationships and social life relatability:43.84%,personal stories and situations:43.65%,fandom in-joke:37.35%,tv and movie reference:36.32%,animals acting like humans:35.82%,abstract or bizarre humour:35.33%</t>
+          <t>funny pet behaviour:44.86%,personal stories and situations:38.24%,genre-reactionary:37.44%,animals acting like humans:37.00%,chaotic low-effort meme:36.33%,referential meme:36.09%</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>mostly larger</t>
+          <t>mostly smaller</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -778,12 +778,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://i.redd.it/v29qg0yrn25g1.jpeg</t>
+          <t>https://i.redd.it/7m9gztd38a5g1.jpeg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/memes/comments/1pdjswx/protect_him_at_all_costs/</t>
+          <t>https://www.reddit.com/r/memes/comments/1peh1jx/its_good_i_guess/</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>35512911</v>
+        <v>35514903</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -816,24 +816,24 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://i.redd.it/v29qg0yrn25g1.jpeg</t>
+          <t>https://i.redd.it/7m9gztd38a5g1.jpeg</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>music and celebrity culture,gender stereotypes,fandom in-joke,job or class stereotypes,culture war discourse,city-specific meme</t>
+          <t>social awkwardness,wholesome animal meme,chaotic low-effort meme,personal stories and situations,everyday inconveniences,referential meme</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://i.redd.it/v29qg0yrn25g1.jpeg</t>
+          <t>https://i.redd.it/7m9gztd38a5g1.jpeg</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/user/Simply_Param/</t>
+          <t>https://www.reddit.com/r/seashanties/comments/gebva4/trying_my_hand_at_this_shanty_meme_thing/</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -846,30 +846,44 @@
           <t>Reddit — discussion communities/subreddits</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>r/seashanties</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>90035</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>smaller</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>technology</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://i.redd.it/6peoynfj0t4g1.jpeg</t>
+          <t>https://i.redd.it/fmtnpvop62x41.png</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>personal stories and situations,relationships and social life relatability,job or class stereotypes,country or region humour,national or ethnic stereotypes,animals acting like humans</t>
+          <t>chaotic low-effort meme,referential meme,abstract or bizarre humour,animal reaction meme,wholesome animal meme,social awkwardness</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://i.redd.it/v29qg0yrn25g1.jpeg</t>
+          <t>https://i.redd.it/7m9gztd38a5g1.jpeg</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/memes/hot/</t>
+          <t>https://www.reddit.com/r/memes/comments/mbw3b0/someone_answer_plz/</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -888,7 +902,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>35512910</v>
+        <v>35514903</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -902,24 +916,24 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/pjrkenkg7wo61.jpg</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>anime and fandom reference,abstract or bizarre humour,fandom in-joke,chaotic low-effort meme,historical figure in modern setting,anti-societal</t>
+          <t>social awkwardness,work or school niche meme,chaotic low-effort meme,referential meme,culture war discourse,abstract or bizarre humour</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://i.redd.it/v29qg0yrn25g1.jpeg</t>
+          <t>https://i.redd.it/7m9gztd38a5g1.jpeg</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/MinecraftMemes/comments/1p6hrzc/capitalism_to_the_end/</t>
+          <t>https://www.reddit.com/r/Funnymemes/comments/1pejbxv/its_good_i_guess/</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -934,11 +948,11 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>r/MinecraftMemes</t>
+          <t>r/Funnymemes</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>3393860</v>
+        <v>1171314</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -952,24 +966,24 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://i.redd.it/bhbdgka0pf3g1.jpeg</t>
+          <t>https://i.redd.it/7c0yyeqyqa5g1.jpeg</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>culture war discourse,music and celebrity culture,gender stereotypes,job or class stereotypes,relationships and social life relatability,internet culture commentary</t>
+          <t>chaotic low-effort meme,wholesome animal meme,animal reaction meme,animals acting like humans,social awkwardness,referential meme</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://i.redd.it/v29qg0yrn25g1.jpeg</t>
+          <t>https://i.redd.it/7m9gztd38a5g1.jpeg</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/MemeTemplatesOfficial/comments/1p4o3gb/the_tech_circle_jerks/</t>
+          <t>https://www.reddit.com/r/meme/comments/1pejdlr/its_good_i_guess/</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -984,11 +998,11 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>r/MemeTemplatesOfficial</t>
+          <t>r/meme</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>388919</v>
+        <v>2806974</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -1002,24 +1016,24 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://i.redd.it/sqwu3sgto03g1.jpeg</t>
+          <t>https://i.redd.it/pcid5txcra5g1.jpeg</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>age group stereotypes,music and celebrity culture,gender stereotypes,job or class stereotypes,culture war discourse,social awkwardness</t>
+          <t>work or school niche meme,chaotic low-effort meme,personal stories and situations,social awkwardness,tv and movie reference,referential meme</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://i.redd.it/v29qg0yrn25g1.jpeg</t>
+          <t>https://i.redd.it/7m9gztd38a5g1.jpeg</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/CATpreparation/comments/1p5kr00/cat_2025_lrdi_arrangement_question_revealed/</t>
+          <t>https://www.reddit.com/r/Funnymemes/comments/1peh08o/i_think_its_good/</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1034,11 +1048,11 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>r/CATpreparation</t>
+          <t>r/Funnymemes</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>289151</v>
+        <v>1171314</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -1047,29 +1061,29 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>technology</t>
+          <t>humor</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://i.redd.it/ykycgdcb883g1.png</t>
+          <t>https://i.redd.it/flz2dq3t7a5g1.jpeg</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>job or class stereotypes,music and celebrity culture,gender stereotypes,age group stereotypes,hobby or niche meme,work or school niche meme</t>
+          <t>chaotic low-effort meme,referential meme,tv and movie reference,social awkwardness,fandom in-joke,work or school niche meme</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://i.redd.it/v29qg0yrn25g1.jpeg</t>
+          <t>https://i.redd.it/7m9gztd38a5g1.jpeg</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/ProgrammerHumor/comments/1p4dzdu/thegang/?tl=en</t>
+          <t>https://www.reddit.com/r/TrollXChromosomes/comments/3x9ips/mfw_my_coworker_keeps_asking_me_questions_and/</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1084,11 +1098,11 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>r/ProgrammerHumor</t>
+          <t>r/TrollXChromosomes</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>4640641</v>
+        <v>834217</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -1097,29 +1111,29 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>technology</t>
+          <t>humor</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://i.redd.it/chzi06astx2g1.jpeg</t>
+          <t>https://i.imgflip.com/897o7.jpg</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>gender stereotypes,job or class stereotypes,social awkwardness,music and celebrity culture,relationships and social life relatability,culture war discourse</t>
+          <t>work or school niche meme,social awkwardness,chaotic low-effort meme,referential meme,animals acting like humans,wholesome animal meme</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://i.redd.it/v29qg0yrn25g1.jpeg</t>
+          <t>https://i.redd.it/7m9gztd38a5g1.jpeg</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/musked/comments/1p4fwkn/a_gaggle_of_cnts/</t>
+          <t>https://www.reddit.com/r/AdviceAnimals/comments/1dfuje6/waving_is_a_terrible_form_of_human_interaction/</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1134,42 +1148,42 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>r/musked</t>
+          <t>r/AdviceAnimals</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>32153</v>
+        <v>9908608</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>smaller</t>
+          <t>larger</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>art</t>
+          <t>niche</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://i.redd.it/pc6nyf66dy2g1.jpeg</t>
+          <t>https://i.redd.it/0g9vrck8ak6d1.jpeg</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>social awkwardness,gender stereotypes,culture war discourse,job or class stereotypes,music and celebrity culture,relationships and social life relatability</t>
+          <t>wholesome animal meme,funny pet behaviour,animal reaction meme,social awkwardness,animals acting like humans,relationships and social life relatability</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://i.redd.it/v29qg0yrn25g1.jpeg</t>
+          <t>https://i.redd.it/7m9gztd38a5g1.jpeg</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/programminghumor/comments/1p9f06l/are_these_guys_friends/</t>
+          <t>https://www.reddit.com/r/Funnymemes/rising/</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1184,11 +1198,11 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>r/programminghumor</t>
+          <t>r/Funnymemes</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>107457</v>
+        <v>1171314</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1202,24 +1216,24 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://i.redd.it/x5dpbp91d44g1.jpeg</t>
+          <t>https://i.redd.it/tskq39qk9e5g1.jpeg</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>music and celebrity culture,referential meme,chronically online behaviour,age group stereotypes,relationships and social life relatability,job or class stereotypes</t>
+          <t>city-specific meme,traditions and heritage humour,culture war discourse,country or region humour,chaotic low-effort meme,relationships and social life relatability</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://i.redd.it/v29qg0yrn25g1.jpeg</t>
+          <t>https://i.redd.it/7m9gztd38a5g1.jpeg</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/BlackboxAI_/comments/1p85nav/naah_chill_bro_we_wont_read_your_messages/</t>
+          <t>https://www.reddit.com/r/AdviceAnimals/comments/8yqno4/overheard_a_couple_at_costco_debating_which/</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1234,42 +1248,42 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>r/BlackboxAI_</t>
+          <t>r/AdviceAnimals</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>19081</v>
+        <v>9908608</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>smaller</t>
+          <t>larger</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>technology</t>
+          <t>niche</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://i.redd.it/6bsabchlnt3g1.jpeg</t>
+          <t>https://i.imgur.com/B12meDR.jpg</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>job or class stereotypes,gender stereotypes,culture war discourse,music and celebrity culture,anti-societal,internet culture commentary</t>
+          <t>referential meme,chaotic low-effort meme,animal reaction meme,work or school niche meme,national or ethnic stereotypes,cross-cultural misunderstanding</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://i.redd.it/a99yc8ehs55g1.jpeg</t>
+          <t>https://i.redd.it/cpomq8u1aa5g1.jpeg</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Brawlstars/comments/1oo9q3a/hopefully_this_will_age_well/</t>
+          <t>https://www.reddit.com/r/gamedev/comments/1dlf13m/5_hard_to_swallow_pills_for_better_game/</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1284,11 +1298,11 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>r/Brawlstars</t>
+          <t>r/gamedev</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>1390262</v>
+        <v>1948433</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1302,24 +1316,24 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://i.redd.it/s9dgl9q0b9zf1.png</t>
+          <t>https://external-preview.redd.it/6HET-8mobSZ-qJKDCpxoI0DXhkvpDrinKqOKlRZmuJo.jpg?auto=webp&amp;s=04c8b8f84e1ec6603205457f6b4533de44718fc9</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>fandom in-joke,culture war discourse,age group stereotypes,historical figure in modern setting,anime and fandom reference,abstract or bizarre humour</t>
+          <t>ideological or partisan conflict,everyday inconveniences,chaotic low-effort meme,cross-cultural misunderstanding,geopolitics and international relations,internet niche meme</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://i.redd.it/a99yc8ehs55g1.jpeg</t>
+          <t>https://i.redd.it/cpomq8u1aa5g1.jpeg</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Cuphead/comments/73puu5/when_you_first_start_dating_vs_6_months_into_the/</t>
+          <t>https://www.reddit.com/r/quantitysurveying/comments/1h6gx7d/what_are_some_hard_truth_pills_about_quantity/</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1334,42 +1348,42 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>r/Cuphead</t>
+          <t>r/quantitysurveying</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>135139</v>
+        <v>7825</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>larger</t>
+          <t>smaller</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>technology</t>
+          <t>music</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://i.redd.it/4951d9igmbpz.jpg</t>
+          <t>https://i.redd.it/htrlr7nqau4e1.png</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>wholesome animal meme,culture war discourse,relationships and social life relatability,abstract or bizarre humour,animal reaction meme,music and celebrity culture</t>
+          <t>everyday inconveniences,abstract or bizarre humour,chaotic low-effort meme,internet niche meme,exhausted,ideological or partisan conflict</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://i.redd.it/a99yc8ehs55g1.jpeg</t>
+          <t>https://i.redd.it/cpomq8u1aa5g1.jpeg</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/enfj/comments/jcjwti/i_try_to_challenge_myself_with_more_enfj_memes/</t>
+          <t>https://www.reddit.com/r/TheMatpatEffect/comments/1nrxsah/the_original_image_of_the_hard_to_swallow_pills/</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1384,11 +1398,11 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>r/enfj</t>
+          <t>r/TheMatpatEffect</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>46790</v>
+        <v>81196</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1402,24 +1416,24 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://i.redd.it/67sf0iu3cjt51.jpg</t>
+          <t>https://preview.redd.it/7pjvu1er4qrf1.jpg?width=640&amp;format=pjpg&amp;auto=webp&amp;s=a252dd57e5b20a9c339d67a2479bdcdf06f6a6e6</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>wholesome animal meme,culture war discourse,animal reaction meme,abstract or bizarre humour,chaotic low-effort meme,traditions and heritage humour</t>
+          <t>internet niche meme,historical figure in modern setting,geopolitics and international relations,tv and movie reference,referential meme,chaotic low-effort meme</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://i.redd.it/a99yc8ehs55g1.jpeg</t>
+          <t>https://i.redd.it/cpomq8u1aa5g1.jpeg</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Cuphead/comments/wau4q3/since_everyone_else_is_doing_it_who_is_this_wrong/</t>
+          <t>https://www.reddit.com/r/smallbusinessuk/comments/1gvp7s4/what_are_some_hard_pills_of_truths_about_running/</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1434,42 +1448,42 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>r/Cuphead</t>
+          <t>r/smallbusinessuk</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>135139</v>
+        <v>55723</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>larger</t>
+          <t>smaller</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>technology</t>
+          <t>art</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>https://i.redd.it/lictikvygfe91.png</t>
+          <t>https://i.redd.it/7t6savgp322e1.png</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>abstract or bizarre humour,referential meme,music and celebrity culture,culture war discourse,historical figure in modern setting,fandom in-joke</t>
+          <t>ideological or partisan conflict,everyday inconveniences,music and celebrity culture,abstract or bizarre humour,culture war discourse,cross-cultural misunderstanding</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://i.redd.it/a99yc8ehs55g1.jpeg</t>
+          <t>https://i.redd.it/cpomq8u1aa5g1.jpeg</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Omorimemes/comments/1jtd3tq/random_title/</t>
+          <t>https://www.reddit.com/r/MoveToScotland/comments/1h2gni7/what_are_the_hard_truths_about_moving_to_scotland/</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1484,11 +1498,11 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>r/Omorimemes</t>
+          <t>r/MoveToScotland</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>26481</v>
+        <v>10204</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1497,29 +1511,29 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>humor</t>
+          <t>niche</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>https://preview.redd.it/w3pxmyk4dcte1.jpg?width=1000&amp;format=pjpg&amp;auto=webp&amp;s=0beacdffe1d494cb73d4288195d43995ce403f85</t>
+          <t>https://i.redd.it/7n4j9qnjos3e1.jpeg</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>wholesome animal meme,animal reaction meme,animals acting like humans,mood relatability,tv and movie reference,funny pet behaviour</t>
+          <t>regional stereotypes,cross-cultural misunderstanding,national or ethnic stereotypes,everyday inconveniences,age group stereotypes,ideological or partisan conflict</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://i.redd.it/a99yc8ehs55g1.jpeg</t>
+          <t>https://i.redd.it/cpomq8u1aa5g1.jpeg</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/armwrestling/comments/1oxt7ri/we_all_know_the_truth/</t>
+          <t>https://www.reddit.com/r/freefolk/comments/96crlp/hard_pills_to_swallow/</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1534,42 +1548,42 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>r/armwrestling</t>
+          <t>r/freefolk</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>37574</v>
+        <v>1276746</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>smaller</t>
+          <t>larger</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>art</t>
+          <t>technology</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>https://i.redd.it/6cj2xo3amf1g1.jpeg</t>
+          <t>https://i.redd.it/5bnz1nsc9df11.png</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>culture war discourse,internet culture commentary,ideological or partisan conflict,music and celebrity culture,domestic politics meme,historical reference meme</t>
+          <t>tv and movie reference,national or ethnic stereotypes,internet niche meme,fandom in-joke,referential meme,historical figure in modern setting</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://i.redd.it/a99yc8ehs55g1.jpeg</t>
+          <t>https://i.redd.it/cpomq8u1aa5g1.jpeg</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/mac/comments/1nqve4z/improper_rounded_corner_alignment/</t>
+          <t>https://www.reddit.com/r/ParamedicsUK/comments/1h122qg/what_are_some_hard_pills_of_truth_when_it_comes/</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1584,42 +1598,42 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>r/mac</t>
+          <t>r/ParamedicsUK</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>2961037</v>
+        <v>16627</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>larger</t>
+          <t>smaller</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>niche</t>
+          <t>lifestyle</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>https://i.redd.it/cq822rvftgrf1.jpeg</t>
+          <t>https://i.redd.it/ntgl8bllhf3e1.png</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>historical figure in modern setting,everyday inconveniences,mood relatability,chaotic low-effort meme,personal failure,meme culture</t>
+          <t>ideological or partisan conflict,everyday inconveniences,referential meme,internet niche meme,tv and movie reference,historical figure in modern setting</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://i.redd.it/a99yc8ehs55g1.jpeg</t>
+          <t>https://i.redd.it/cpomq8u1aa5g1.jpeg</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Cuphead/comments/17e1u6s/cute_flower/</t>
+          <t>https://www.reddit.com/r/NOTHING/comments/1m36exo/not_liking_the_nothing_phone_3_may_mean_accepting/</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1634,15 +1648,15 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>r/Cuphead</t>
+          <t>r/NOTHING</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>135139</v>
+        <v>70583</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>larger</t>
+          <t>smaller</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1652,24 +1666,24 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>https://i.redd.it/xibpwx0z7tvb1.jpg</t>
+          <t>https://i.redd.it/znjtvq2jpndf1.jpeg</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>wholesome animal meme,historical figure in modern setting,animal reaction meme,animals acting like humans,abstract or bizarre humour,fandom in-joke</t>
+          <t>everyday inconveniences,personal stories and situations,gender stereotypes,anti-societal,internet culture commentary,abstract or bizarre humour</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://i.redd.it/a99yc8ehs55g1.jpeg</t>
+          <t>https://i.redd.it/cpomq8u1aa5g1.jpeg</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/PlantsVSZombies/comments/1ivf25w/lightning_reed_meme/</t>
+          <t>https://www.reddit.com/r/irishpolitics/comments/1oisa2r/hard_to_swallow_pills_and_the_race_for_irish/</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1684,42 +1698,42 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>r/PlantsVSZombies</t>
+          <t>r/irishpolitics</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>153734</v>
+        <v>25866</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>larger</t>
+          <t>smaller</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>gaming</t>
+          <t>political</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>https://i.redd.it/5o81q0vatnke1.jpeg</t>
+          <t>https://external-preview.redd.it/qGTxzdi2GiN6An6RrglH3OyOoKPjoSTfU_vtvwlfmpM.jpeg?auto=webp&amp;s=d974444a0db5b88339bdca2d2a9186da2e1044a5</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>abstract or bizarre humour,funny pet behaviour,tv and movie reference,animal reaction meme,chaotic low-effort meme,referential meme</t>
+          <t>national or ethnic stereotypes,ideological or partisan conflict,culture war discourse,cross-cultural misunderstanding,historical figure in modern setting,chaotic low-effort meme</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://i.redd.it/a99yc8ehs55g1.jpeg</t>
+          <t>https://i.redd.it/cpomq8u1aa5g1.jpeg</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/TwentiesIndia/comments/1nk17lk/imagine/</t>
+          <t>https://www.reddit.com/r/h3h3productions/comments/15wyrim/learning_to_enjoy_what_we_have_right_now/</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1734,11 +1748,11 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>r/TwentiesIndia</t>
+          <t>r/h3h3productions</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>124144</v>
+        <v>585609</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1747,21 +1761,29 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>niche</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
+          <t>humor</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z03t2sh2lejb1.jpg</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>historical figure in modern setting,tv and movie reference,abstract or bizarre humour,chaotic low-effort meme,music and celebrity culture,fandom in-joke</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://i.redd.it/wdlamvzy015g1.png</t>
+          <t>https://i.redd.it/536z12131a5g1.jpeg</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/wow/comments/k19vb0/me_10_seconds_after_trying_to_use_my_mount_in_the/</t>
+          <t>https://www.reddit.com/r/memes/comments/1peg5a7/just_a_quick_trip/</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1776,11 +1798,11 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>r/wow</t>
+          <t>r/memes</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>3063813</v>
+        <v>35514906</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1789,29 +1811,29 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>gaming</t>
+          <t>humor</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>https://i.redd.it/kd55tb911j161.jpg</t>
+          <t>https://i.redd.it/536z12131a5g1.jpeg</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>animals acting like humans,wholesome animal meme,animal reaction meme,historical figure in modern setting,traditions and heritage humour,funny pet behaviour</t>
+          <t>chaotic low-effort meme,relationships and social life relatability,culture war discourse,abstract or bizarre humour,referential meme,internet niche meme</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://i.redd.it/wdlamvzy015g1.png</t>
+          <t>https://i.redd.it/536z12131a5g1.jpeg</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/AssassinsCreedValhala/comments/nfky0v/everybody_god_i_hate_fishing_to_do_altar/</t>
+          <t>https://www.reddit.com/r/dankmemes/comments/u2qfk9/meme/</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1826,11 +1848,11 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>r/AssassinsCreedValhala</t>
+          <t>r/dankmemes</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>124955</v>
+        <v>5848558</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1839,29 +1861,29 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>niche</t>
+          <t>humor</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>https://i.redd.it/60kvfh1hsxz61.jpg</t>
+          <t>https://i.redd.it/uq922u1utat81.jpg</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>animals acting like humans,wholesome animal meme,funny pet behaviour,animal reaction meme,historical figure in modern setting,fandom in-joke</t>
+          <t>personal failure,gaming pop culture joke,culture war discourse,anti-societal,fandom in-joke,chaotic low-effort meme</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://i.redd.it/wdlamvzy015g1.png</t>
+          <t>https://i.redd.it/536z12131a5g1.jpeg</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/footballmanagergames/comments/xpbhny/my_instructions_much_shorter_passing_pass_to_cb/</t>
+          <t>https://www.reddit.com/r/memes/comments/gcp0d4/cries_in_different_time_zone/</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1876,11 +1898,11 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>r/footballmanagergames</t>
+          <t>r/memes</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>512108</v>
+        <v>35514906</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1889,29 +1911,29 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>gaming</t>
+          <t>humor</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>https://i.redd.it/v7t7p4qradq91.jpg</t>
+          <t>https://i.redd.it/3cc0tdjlbjw41.jpg</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>animals acting like humans,wholesome animal meme,animal reaction meme,traditions and heritage humour,historical figure in modern setting,funny pet behaviour</t>
+          <t>historical figure in modern setting,meme culture,animals acting like humans,culture war discourse,chaotic low-effort meme,genre-reactionary</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://i.redd.it/wdlamvzy015g1.png</t>
+          <t>https://i.redd.it/536z12131a5g1.jpeg</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Accounting/comments/1iv7pwn/me_looking_at_the_budget_this_year_after_blowing/</t>
+          <t>https://www.reddit.com/r/memes/comments/1pep9mq/can_someone_pls_help_me_find_the_meme_where_man/</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1926,11 +1948,11 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>r/Accounting</t>
+          <t>r/memes</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>1190320</v>
+        <v>35514906</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1939,29 +1961,29 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>finance</t>
+          <t>humor</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>https://i.redd.it/34yrykliklke1.jpeg</t>
+          <t>https://i.redd.it/grhbnwfccc5g1.jpeg</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>animals acting like humans,wholesome animal meme,tv and movie reference,referential meme,animal reaction meme,historical figure in modern setting</t>
+          <t>personal failure,historical figure in modern setting,internet niche meme,hobby or niche meme,chaotic low-effort meme,animals acting like humans</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://i.redd.it/wdlamvzy015g1.png</t>
+          <t>https://i.redd.it/536z12131a5g1.jpeg</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/GodofWar/comments/s3ff1n/choosing_to_suffer_through_give_me_god_of_war/</t>
+          <t>https://www.reddit.com/r/memes/comments/r7tigg/so_complicated/</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1976,11 +1998,11 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>r/GodofWar</t>
+          <t>r/memes</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>452479</v>
+        <v>35514905</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1989,29 +2011,29 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>technology</t>
+          <t>humor</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>https://i.redd.it/5lwc2py02kb81.jpg</t>
+          <t>https://i.redd.it/max4vhy45a381.gif</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>animals acting like humans,wholesome animal meme,funny pet behaviour,animal reaction meme,chaotic low-effort meme,fandom in-joke</t>
+          <t>work or school niche meme,personal stories and situations,tv and movie reference,traditions and heritage humour,meme culture,chaotic low-effort meme</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://i.redd.it/wdlamvzy015g1.png</t>
+          <t>https://i.redd.it/536z12131a5g1.jpeg</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/foxholegame/comments/ygrbs7/charlie_wasted_a_nuke_for_clout_stupid_target_low/</t>
+          <t>https://www.reddit.com/r/meme/comments/gg59o5/still_refreshing/</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2026,42 +2048,42 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>r/foxholegame</t>
+          <t>r/meme</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>96679</v>
+        <v>2806976</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>smaller</t>
+          <t>larger</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>gaming</t>
+          <t>humor</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>https://i.redd.it/kwjv0a74isw91.png</t>
+          <t>https://i.redd.it/v5h6x3yswmx41.jpg</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>wholesome animal meme,animals acting like humans,funny pet behaviour,animal reaction meme,age group stereotypes,referential meme</t>
+          <t>social awkwardness,meme culture,chaotic low-effort meme,genre-reactionary,mood relatability,personal stories and situations</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://i.redd.it/wdlamvzy015g1.png</t>
+          <t>https://i.redd.it/536z12131a5g1.jpeg</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Thunder/comments/1i8mocn/mark_when_you_beg_him_to_play_caruso_instead_of/</t>
+          <t>https://www.reddit.com/r/PeterExplainsTheJoke/comments/1pf5hyz/petah/</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2076,11 +2098,11 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>r/Thunder</t>
+          <t>r/PeterExplainsTheJoke</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>526704</v>
+        <v>2956844</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -2089,29 +2111,29 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>sports</t>
+          <t>humor</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>https://i.redd.it/xykrcp4z6vee1.jpeg</t>
+          <t>https://i.redd.it/bca5nbep1g5g1.jpeg</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>animals acting like humans,wholesome animal meme,animal reaction meme,referential meme,funny pet behaviour,historical figure in modern setting</t>
+          <t>chaotic low-effort meme,animals acting like humans,referential meme,genre-reactionary,funny pet behaviour,historical figure in modern setting</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://i.redd.it/wdlamvzy015g1.png</t>
+          <t>https://i.redd.it/536z12131a5g1.jpeg</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Gunners/comments/1junxoi/declan_rice_lining_up_for_the_second_free_kick/</t>
+          <t>https://www.reddit.com/r/DeathBattleMatchups/comments/11swbeb/me_refreshing_my_tab_and_waiting_for_bread_to/</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2126,15 +2148,15 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>r/Gunners</t>
+          <t>r/DeathBattleMatchups</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>505394</v>
+        <v>46839</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>larger</t>
+          <t>smaller</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2144,24 +2166,24 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>https://external-preview.redd.it/ZOHOS0pwWERkug4K_sosAoAhsTrRSmDKNbEbp2fkTf8.jpg?auto=webp&amp;s=3a8304593c59e06e624f1ba44a6871a2a2e6cfa1</t>
+          <t>https://i.redd.it/6ef119bz54oa1.jpg</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>wholesome animal meme,animals acting like humans,funny pet behaviour,animal reaction meme,referential meme,culture war discourse</t>
+          <t>animals acting like humans,historical figure in modern setting,chaotic low-effort meme,fandom in-joke,relationships and social life relatability,exhausted</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://i.redd.it/wdlamvzy015g1.png</t>
+          <t>https://i.redd.it/536z12131a5g1.jpeg</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/canucks/comments/1hx3ghe/myers_passing_in_ot/</t>
+          <t>https://www.reddit.com/r/Maplestory/comments/3h5kod/price_check_would_you_buy_this_claw/</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2176,11 +2198,11 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>r/canucks</t>
+          <t>r/Maplestory</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>198664</v>
+        <v>140647</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -2194,24 +2216,24 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>https://i.redd.it/ktos50wszvbe1.jpeg</t>
+          <t>https://external-preview.redd.it/LYnpO0oDcKw12tEJr9-WVftx_y2W_XCUvpu3q64BFEs.jpg?auto=webp&amp;s=dea21f71098b0ba7ce3f9e5849d2a006dacb2438</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>wholesome animal meme,animals acting like humans,animal reaction meme,funny pet behaviour,mood relatability,historical figure in modern setting</t>
+          <t>exhausted,internet niche meme,wholesome animal meme,fandom in-joke,anime and fandom reference,chaotic low-effort meme</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://i.redd.it/wdlamvzy015g1.png</t>
+          <t>https://i.redd.it/536z12131a5g1.jpeg</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Bannerlord/comments/1if47y2/but_sire_the_lord_you_just_executed_was/</t>
+          <t>https://www.reddit.com/r/memes/comments/jb3ri2/i_keep_refreshing/</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2226,11 +2248,11 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>r/Bannerlord</t>
+          <t>r/memes</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>220686</v>
+        <v>35514906</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -2239,29 +2261,29 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>niche</t>
+          <t>humor</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>https://i.redd.it/vdoqn1b9hige1.jpeg</t>
+          <t>https://i.redd.it/6h2xj0m253t51.png</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>animals acting like humans,wholesome animal meme,animal reaction meme,funny pet behaviour,historical figure in modern setting,mood relatability</t>
+          <t>anime and fandom reference,genre-reactionary,animals acting like humans,personal stories and situations,chaotic low-effort meme,personal failure</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/tufn98a4hc5g1.png</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/memes/</t>
+          <t>https://www.reddit.com/r/memes/comments/1pepp0n/what_its_like_to_solve_trigonometry_problems/</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2280,7 +2302,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>35512915</v>
+        <v>35514906</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -2294,24 +2316,24 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/tufn98a4hc5g1.png</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>abstract or bizarre humour,chaotic low-effort meme,tv and movie reference,referential meme,fandom in-joke,funny pet behaviour</t>
+          <t>everyday inconveniences,internet niche meme,chaotic low-effort meme,abstract or bizarre humour,animal reaction meme,exhausted</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/tufn98a4hc5g1.png</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/memes/comments/1pdy2c5/way_down_we_go/</t>
+          <t>https://www.reddit.com/r/memes/hot/</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2330,7 +2352,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>35512916</v>
+        <v>35514906</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -2344,24 +2366,24 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/eehpu246me5g1.png</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>tv and movie reference,abstract or bizarre humour,chaotic low-effort meme,referential meme,genre-reactionary,internet niche meme</t>
+          <t>historical figure in modern setting,chaotic low-effort meme,social awkwardness,genre-reactionary,gender stereotypes,personal stories and situations</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/n77t88wpob5g1.jpeg</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/t/memes/</t>
+          <t>https://www.reddit.com/r/IronWarriors/comments/1m5fwzj/in_need_of_a_iron_warriors_expert/</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2374,22 +2396,44 @@
           <t>Reddit — discussion communities/subreddits</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>r/IronWarriors</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>43933</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>smaller</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>technology</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhk5i0jrl7ef1.jpeg</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>funny pet behaviour,animal reaction meme,animals acting like humans,fandom in-joke,wholesome animal meme,job or class stereotypes</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/n77t88wpob5g1.jpeg</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/XGramatikInsights/comments/1o6ed5c/global_markets_right_now_not_this_sht_again/</t>
+          <t>https://www.reddit.com/r/MePettingMyCat/comments/n4ejdd/me_petting_my_cat_after_i_erased_the_background/</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2404,34 +2448,42 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>r/XGramatikInsights</t>
+          <t>r/MePettingMyCat</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>197753</v>
+        <v>4573</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>larger</t>
+          <t>smaller</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>finance</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
+          <t>humor</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mtrstuhnm0x61.png</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>funny pet behaviour,animals acting like humans,wholesome animal meme,animal reaction meme,chaotic low-effort meme,meme culture</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/n77t88wpob5g1.jpeg</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Ontario_Sub/comments/1mfw0or/us_senator_canada_is_the_largest_trading_partner/</t>
+          <t>https://www.reddit.com/r/DrewDurnil/comments/1dr7oyk/can_someone_make_this_cat_look_like_kim_jong_un/</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2446,11 +2498,11 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>r/Ontario_Sub</t>
+          <t>r/DrewDurnil</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>2231</v>
+        <v>68595</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -2459,21 +2511,29 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>political</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
+          <t>niche</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzze1yv9gh9d1.png</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>animals acting like humans,funny pet behaviour,wholesome animal meme,animal reaction meme,music and celebrity culture,referential meme</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/n77t88wpob5g1.jpeg</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/t/internet_culture/</t>
+          <t>https://www.reddit.com/r/DankMemesFromSite19/comments/pepshi/i_dont_know_why_but_scp607_feels_both_wholesome/</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2486,22 +2546,44 @@
           <t>Reddit — discussion communities/subreddits</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>r/DankMemesFromSite19</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>230079</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>larger</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>humor</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5i5chk4wjk71.jpg</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>funny pet behaviour,wholesome animal meme,animals acting like humans,chaotic low-effort meme,culture war discourse,music and celebrity culture</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/n77t88wpob5g1.jpeg</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/MAXNSQUEEZE/comments/1f272as/shareholder_alert_pomerantz_law_firm_announces/</t>
+          <t>https://www.reddit.com/r/DeathBattleMatchups/comments/1hi5oql/me_caressing_the_new_matchup_i_like_before_its/</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2516,11 +2598,11 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>r/MAXNSQUEEZE</t>
+          <t>r/DeathBattleMatchups</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>2341</v>
+        <v>46839</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -2532,18 +2614,26 @@
           <t>niche</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/isgo0we2zv7e1.jpeg</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>funny pet behaviour,animals acting like humans,wholesome animal meme,animal reaction meme,culture war discourse,music and celebrity culture</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/n77t88wpob5g1.jpeg</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/RobinHoodPennyStocks/comments/lsxukw/the_last_two_weeks/</t>
+          <t>https://www.reddit.com/r/memes/comments/o1qjdn/i_miss_it_tbh/</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2558,11 +2648,11 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>r/RobinHoodPennyStocks</t>
+          <t>r/memes</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>615025</v>
+        <v>35514906</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -2571,21 +2661,29 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>finance</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr"/>
+          <t>humor</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ismyloyptr571.jpg</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>animal reaction meme,animals acting like humans,funny pet behaviour,wholesome animal meme,chaotic low-effort meme,genre-reactionary</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/n77t88wpob5g1.jpeg</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/ConeHeads/comments/1e8wbqm/why_the_recent_dip/</t>
+          <t>https://www.reddit.com/r/PcBuild/comments/1pby8v0/was_the_car_worth_it/</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2600,34 +2698,42 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>r/ConeHeads</t>
+          <t>r/PcBuild</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>17012</v>
+        <v>640453</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>smaller</t>
+          <t>larger</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>niche</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr"/>
+          <t>gaming</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4j6zo62qp4g1.jpeg</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>funny pet behaviour,wholesome animal meme,animals acting like humans,personal stories and situations,meme culture,personal failure</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
+          <t>https://i.redd.it/n77t88wpob5g1.jpeg</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/Trumpvirus/comments/1jrg0wq/maga_in_2025/</t>
+          <t>https://www.reddit.com/r/GODZILLA/comments/178z4eq/who_wins/</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2642,34 +2748,36 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>r/Trumpvirus</t>
-        </is>
-      </c>
-      <c r="F41" t="n">
-        <v>98835</v>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>smaller</t>
-        </is>
-      </c>
+          <t>r/GODZILLA</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>political</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
+          <t>niche</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>https://preview.redd.it/fdm8g2y97iub1.jpg?width=647&amp;format=pjpg&amp;auto=webp&amp;s=9d4c7462107bd47e65a9463d2d0736a28ffc67dd</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>fandom in-joke,abstract or bizarre humour,referential meme,age group stereotypes,anime and fandom reference,tv and movie reference</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://i.redd.it/eqlv3h9rb15g1.png</t>
+          <t>https://i.redd.it/n77t88wpob5g1.jpeg</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/memes/comments/1pdcsfu/dinner_is_cooked_lets_eat/</t>
+          <t>https://www.reddit.com/r/memes/comments/1c0eu5r/cant_help_but_love_them/</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2687,39 +2795,25 @@
           <t>r/memes</t>
         </is>
       </c>
-      <c r="F42" t="n">
-        <v>35512917</v>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>larger</t>
-        </is>
-      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
           <t>humor</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>https://i.redd.it/eqlv3h9rb15g1.png</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>personal stories and situations,tv and movie reference,relationships and social life relatability,meme culture,gender stereotypes,animals acting like humans</t>
-        </is>
-      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://i.redd.it/eqlv3h9rb15g1.png</t>
+          <t>https://i.redd.it/n77t88wpob5g1.jpeg</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://www.reddit.com/r/JEENEETards/comments/1pd2q8t/advice_for_maths/</t>
+          <t>https://www.reddit.com/r/memes/comments/1pen392/why_ram_prices_shooting_up_lately/</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2734,132 +2828,18 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>r/JEENEETards</t>
-        </is>
-      </c>
-      <c r="F43" t="n">
-        <v>498336</v>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>larger</t>
-        </is>
-      </c>
+          <t>r/memes</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>art</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>https://i.redd.it/54vv4d93fz4g1.png</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>anime and fandom reference,relationships and social life relatability,fandom in-joke,abstract or bizarre humour,personal stories and situations,tv and movie reference</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>https://i.redd.it/eqlv3h9rb15g1.png</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/memes/hot/</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Reddit - The heart of the internet</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Reddit — discussion communities/subreddits</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>r/memes</t>
-        </is>
-      </c>
-      <c r="F44" t="n">
-        <v>35512917</v>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>larger</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
           <t>humor</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>https://i.redd.it/u5ixyww8e65g1.gif</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>abstract or bizarre humour,anime and fandom reference,referential meme,genre-reactionary,chaotic low-effort meme,music and celebrity culture</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>https://i.redd.it/eqlv3h9rb15g1.png</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>https://www.reddit.com/r/JEENEETards/rising/</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Reddit - The heart of the internet</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Reddit — discussion communities/subreddits</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>r/JEENEETards</t>
-        </is>
-      </c>
-      <c r="F45" t="n">
-        <v>498336</v>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>larger</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>art</t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>https://i.redd.it/zd5wu5b0x65g1.jpeg</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>relationships and social life relatability,chronically online behaviour,gender stereotypes,funny pet behaviour,wholesome animal meme,social awkwardness</t>
-        </is>
-      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>